<commit_message>
Sudah lengkap nomor WAnya
</commit_message>
<xml_diff>
--- a/2026.xlsx
+++ b/2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\jadwal-imam-tarawih\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA1C73B-18DD-41B0-A681-AAED6AEC66A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9242A2A-FB2D-4809-9B2E-279696D518E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="146">
   <si>
     <t>Jadwal Petugas Kegiatan Tarawih Ramadhan 1446 H</t>
   </si>
@@ -461,6 +461,30 @@
   </si>
   <si>
     <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Di DT</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>Nomor WA</t>
+  </si>
+  <si>
+    <t>+62 821-5344-2363</t>
+  </si>
+  <si>
+    <t>+62 853-4675-1595</t>
+  </si>
+  <si>
+    <t>Ustadz Rahmad</t>
+  </si>
+  <si>
+    <t>+62 813-4632-6451</t>
+  </si>
+  <si>
+    <t>+62 852-4876-8450</t>
   </si>
 </sst>
 </file>
@@ -507,7 +531,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -530,13 +554,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -576,38 +611,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -617,6 +640,52 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-421]dddd&quot;, &quot;dd\ mmmm\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -635,15 +704,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -683,15 +752,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -731,15 +800,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -769,7 +838,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12363450" y="952500"/>
+          <a:off x="9744075" y="0"/>
           <a:ext cx="6343650" cy="6715125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -780,6 +849,22 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F672EF5-F5A6-4182-8647-3A86B3566FAB}" name="Table1" displayName="Table1" ref="A5:E34" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A5:E34" xr:uid="{7F672EF5-F5A6-4182-8647-3A86B3566FAB}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{EDA3354A-D911-4857-BDFD-2A76F68799B6}" name="Nomor" dataDxfId="3">
+      <calculatedColumnFormula>A5+1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{EE32957E-B020-43A5-93B6-4F4983A5B8C5}" name="Tanggal" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{474FEB94-AA9D-4225-84A8-CAE68BC78718}" name="Imam"/>
+    <tableColumn id="4" xr3:uid="{E9CF7577-A218-4BFC-BD73-D8F2523F2B45}" name="Keterangan"/>
+    <tableColumn id="5" xr3:uid="{11BF8C20-01CD-49CD-96D6-A73B48384BCF}" name="Nomor WA"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1040,748 +1125,1124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A2:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="26.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.7109375" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="12" t="s">
+    <row r="2" spans="1:10">
+      <c r="A2" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="1"/>
-      <c r="F1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="I3" s="20"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="13" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="J2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="I4" s="19"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="16">
+      <c r="E5" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="14">
         <v>1</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16" t="s">
+      <c r="B6" s="15">
+        <v>46071</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="I5" s="19" t="s">
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="16">
-        <f t="shared" ref="A6:A33" si="0">A5+1</f>
+    <row r="7" spans="1:10">
+      <c r="A7" s="14">
+        <f t="shared" ref="A7:A34" si="0">A6+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16" t="s">
+      <c r="B7" s="15">
+        <v>46072</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="I6" s="19" t="s">
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="16">
+    <row r="8" spans="1:10">
+      <c r="A8" s="14">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16" t="s">
+      <c r="B8" s="15">
+        <v>46073</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="I7" s="19" t="s">
+      <c r="G8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="16">
+    <row r="9" spans="1:10">
+      <c r="A9" s="14">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16" t="s">
+      <c r="B9" s="15">
+        <v>46074</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>139</v>
+      </c>
+      <c r="J9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B10" s="15">
+        <v>46075</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="I8" s="19" t="s">
+      <c r="G10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B11" s="15">
+        <v>46076</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
+        <v>132</v>
+      </c>
+      <c r="J11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B12" s="15">
+        <v>46077</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B13" s="15">
+        <v>46078</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="14">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B14" s="15">
+        <v>46079</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" t="s">
+        <v>135</v>
+      </c>
+      <c r="J14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B15" s="15">
+        <v>46080</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="16">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16" t="s">
+      <c r="J15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="14">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B16" s="15">
+        <v>46081</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B17" s="15">
+        <v>46082</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" t="s">
+        <v>131</v>
+      </c>
+      <c r="J17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B18" s="15">
+        <v>46083</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" t="s">
+        <v>101</v>
+      </c>
+      <c r="J18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="14">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B19" s="15">
+        <v>46084</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B20" s="15">
+        <v>46085</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" t="s">
+        <v>71</v>
+      </c>
+      <c r="J20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B21" s="15">
+        <v>46086</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" t="s">
+        <v>128</v>
+      </c>
+      <c r="J21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="14">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B22" s="15">
+        <v>46087</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="14">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B23" s="15">
+        <v>46088</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="14">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="15">
+        <v>46089</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B25" s="15">
+        <v>46090</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" t="s">
+        <v>135</v>
+      </c>
+      <c r="J25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="14">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B26" s="15">
+        <v>46091</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="14">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B27" s="15">
+        <v>46092</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="14">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B28" s="15">
+        <v>46093</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="16"/>
+      <c r="E28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" t="s">
+        <v>86</v>
+      </c>
+      <c r="H28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="14">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B29" s="15">
+        <v>46094</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="I9" s="19" t="s">
+      <c r="G29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="14">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B30" s="15">
+        <v>46095</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="E30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="14">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B31" s="15">
+        <v>46096</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="16">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16" t="s">
+      <c r="D31" s="16"/>
+      <c r="E31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="I10" s="19" t="s">
+      <c r="G31" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="14">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B32" s="15">
+        <v>46097</v>
+      </c>
+      <c r="C32" s="16" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="16">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16" t="s">
+      <c r="D32" s="16"/>
+      <c r="E32" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="I11" s="19" t="s">
+      <c r="G32" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="14">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B33" s="15">
+        <v>46098</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="16"/>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="14">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B34" s="15">
+        <v>46099</v>
+      </c>
+      <c r="C34" s="16" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="16">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="F35" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="J39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="J40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="J41" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="J42" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="J43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="J44" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="J45" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="J46" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="J47" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="I12" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="16">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16" t="s">
+      <c r="K47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="J48" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K48" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="10:11">
+      <c r="J49" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="10:11">
+      <c r="J50" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="10:11">
+      <c r="J51" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="10:11">
+      <c r="J52" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="10:11">
+      <c r="J53" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K53" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="10:11">
+      <c r="J54" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="10:11">
+      <c r="J55" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="10:11">
+      <c r="J56" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="10:11">
+      <c r="J57" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="I13" s="19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="16">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="15"/>
-      <c r="I14" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="16">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="15"/>
-      <c r="I15" s="19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="16">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="15"/>
-      <c r="I16" s="19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="16">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="15"/>
-      <c r="I17" s="19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="16">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="15"/>
-      <c r="I18" s="19" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="15"/>
-      <c r="I19" s="19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16" t="s">
+      <c r="K57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="10:11">
+      <c r="J58" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="10:11">
+      <c r="J59" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="10:11">
+      <c r="J60" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="10:11">
+      <c r="J61" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="10:11">
+      <c r="J62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K62" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="10:11">
+      <c r="J63" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="10:11">
+      <c r="J64" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K64" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="10:11">
+      <c r="J65" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K65" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="10:11">
+      <c r="J66" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="I20" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="16">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="I21" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="16">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="15"/>
-      <c r="I22" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="16">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B23" s="17"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="15"/>
-      <c r="I23" s="19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="16">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="15"/>
-      <c r="I24" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="16">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B25" s="17"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="15"/>
-      <c r="I25" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="16">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B26" s="17"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="15"/>
-      <c r="I26" s="19"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="16">
-        <f t="shared" si="0"/>
+      <c r="K66" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="15"/>
-      <c r="I27" s="19"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="16">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="15"/>
-      <c r="I28" s="19"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="16">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B29" s="17"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="15"/>
-      <c r="I29" s="21"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="16">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B30" s="17"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="15"/>
-      <c r="I30" s="21"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="16">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B31" s="17"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="15"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="16">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B32" s="17"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="15"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="16">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B33" s="17"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="16">
-        <v>30</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="15"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="F39" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="F40" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="F41" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G41" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="F42" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="F43" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="F44" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="F45" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G45" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="F46" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G46" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="F47" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G47" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="F48" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G48" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="6:7">
-      <c r="F49" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="6:7">
-      <c r="F50" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="6:7">
-      <c r="F51" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="6:7">
-      <c r="F52" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" spans="6:7">
-      <c r="F53" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G53" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="6:7">
-      <c r="F54" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="6:7">
-      <c r="F55" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G55" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="56" spans="6:7">
-      <c r="F56" s="16" t="s">
+    </row>
+    <row r="67" spans="10:11">
+      <c r="J67" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G56" s="15" t="s">
+      <c r="K67" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="6:7">
-      <c r="F57" s="16" t="s">
+    <row r="68" spans="10:11">
+      <c r="J68" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G57" s="15" t="s">
+      <c r="K68" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="6:7">
-      <c r="F58" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="59" spans="6:7">
-      <c r="F59" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G59" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="6:7">
-      <c r="F60" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G60" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="6:7">
-      <c r="F61" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G61" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="62" spans="6:7">
-      <c r="F62" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G62" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="63" spans="6:7">
-      <c r="F63" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G63" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="64" spans="6:7">
-      <c r="F64" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G64" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="6:7">
-      <c r="F65" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G65" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="6:7">
-      <c r="F66" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="G66" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="6:7">
-      <c r="F67" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="G67" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="68" spans="6:7">
-      <c r="F68" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G68" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I5:I24">
-    <sortCondition ref="I24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J6:J27">
+    <sortCondition ref="J6:J27"/>
   </sortState>
   <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
   </mergeCells>
+  <conditionalFormatting sqref="H6:H34">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>C6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>